<commit_message>
Added new words to Words.xlsx
continuation working on quiz
</commit_message>
<xml_diff>
--- a/Words.xlsx
+++ b/Words.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\ExVileEs-D\škola\Vejška\My_Projects\NJLearner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MatlabWorkSpace\NJLearner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F95058E-134C-49B5-93F1-47B0D44A1025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04933BD-C3C5-4ECE-BE79-474F3821BA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>die Katze</t>
   </si>
@@ -58,13 +58,84 @@
   </si>
   <si>
     <t>Ceske_slovo</t>
+  </si>
+  <si>
+    <t>slon</t>
+  </si>
+  <si>
+    <r>
+      <t>der</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>Elefant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>die</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>Schildkröte</t>
+    </r>
+  </si>
+  <si>
+    <t>želva</t>
+  </si>
+  <si>
+    <r>
+      <t>der</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> Papagei</t>
+    </r>
+  </si>
+  <si>
+    <t>papoušek</t>
+  </si>
+  <si>
+    <t>kůň</t>
+  </si>
+  <si>
+    <t>das Pferd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,13 +143,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF5F6368"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF5F6368"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,8 +202,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -375,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -394,7 +514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -405,7 +525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -416,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -427,7 +547,51 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added feature of selecting category of Words more over more verbs added to Words.xlsx
</commit_message>
<xml_diff>
--- a/Words.xlsx
+++ b/Words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MatlabWorkSpace\NJLearner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD89B857-3A37-432C-AB91-59C3A14F316B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9E7BC2-C172-44A8-B937-43B1F388AAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>die Katze</t>
   </si>
@@ -140,13 +140,112 @@
     </r>
   </si>
   <si>
-    <t>Pajda</t>
-  </si>
-  <si>
-    <t>das Phajda</t>
-  </si>
-  <si>
-    <t>human</t>
+    <t>jmenovat se</t>
+  </si>
+  <si>
+    <t>heißen</t>
+  </si>
+  <si>
+    <t>prosit</t>
+  </si>
+  <si>
+    <t>bitten</t>
+  </si>
+  <si>
+    <t>přijít</t>
+  </si>
+  <si>
+    <t>kommen</t>
+  </si>
+  <si>
+    <t>(po)těšit</t>
+  </si>
+  <si>
+    <t>freuen</t>
+  </si>
+  <si>
+    <t>děkovat</t>
+  </si>
+  <si>
+    <t>danken</t>
+  </si>
+  <si>
+    <t>dělat - fyzicky?</t>
+  </si>
+  <si>
+    <t>machen</t>
+  </si>
+  <si>
+    <t>doprovázet</t>
+  </si>
+  <si>
+    <t>begleinten</t>
+  </si>
+  <si>
+    <t>studovat</t>
+  </si>
+  <si>
+    <t>studieren</t>
+  </si>
+  <si>
+    <t>besuchen</t>
+  </si>
+  <si>
+    <t>navštívit</t>
+  </si>
+  <si>
+    <t>bydlet</t>
+  </si>
+  <si>
+    <t>wohnen</t>
+  </si>
+  <si>
+    <t>říkat</t>
+  </si>
+  <si>
+    <t>sagen</t>
+  </si>
+  <si>
+    <t>představovat</t>
+  </si>
+  <si>
+    <t>vorstellen</t>
+  </si>
+  <si>
+    <t>arbeiten</t>
+  </si>
+  <si>
+    <t>dělat</t>
+  </si>
+  <si>
+    <t>wandern</t>
+  </si>
+  <si>
+    <t>chodit na tůry</t>
+  </si>
+  <si>
+    <t>kutit</t>
+  </si>
+  <si>
+    <t>basteln</t>
+  </si>
+  <si>
+    <t>dělat/činit</t>
+  </si>
+  <si>
+    <t>tun</t>
+  </si>
+  <si>
+    <t>učit se</t>
+  </si>
+  <si>
+    <t>lernen</t>
+  </si>
+  <si>
+    <t>plavat</t>
+  </si>
+  <si>
+    <t>schwimmen</t>
   </si>
 </sst>
 </file>
@@ -485,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -594,7 +693,194 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Přidání nových možností quizu úprava slov
</commit_message>
<xml_diff>
--- a/Words.xlsx
+++ b/Words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MatlabWorkSpace\NJLearner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550FF22F-F18D-43AB-A71E-FDE059C8C7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB406B5-C578-4317-9869-66C72D19CBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
   <si>
     <t>die Katze</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>gehen</t>
-  </si>
-  <si>
-    <t>sloveso</t>
   </si>
   <si>
     <t>pes</t>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>sehen</t>
+  </si>
+  <si>
+    <t>verbs</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,13 +742,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -775,21 +775,21 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -797,10 +797,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -808,10 +808,10 @@
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -820,10 +820,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -831,391 +831,463 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
         <v>51</v>
       </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
         <v>55</v>
       </c>
-      <c r="B27" t="s">
-        <v>56</v>
+      <c r="C27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="B28" t="s">
-        <v>58</v>
+      <c r="C28" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
         <v>59</v>
       </c>
-      <c r="B29" t="s">
-        <v>60</v>
+      <c r="C29" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
         <v>61</v>
       </c>
-      <c r="B30" t="s">
-        <v>62</v>
+      <c r="C30" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
         <v>63</v>
       </c>
-      <c r="B31" t="s">
-        <v>64</v>
+      <c r="C31" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>67</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>72</v>
       </c>
-      <c r="B35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>73</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>75</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>77</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>79</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>81</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>86</v>
       </c>
-      <c r="B42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>87</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>89</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>92</v>
       </c>
-      <c r="B45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>93</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>95</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>97</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
         <v>99</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
         <v>101</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More Words.xlsx added corretion
</commit_message>
<xml_diff>
--- a/Words.xlsx
+++ b/Words.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MatlabWorkSpace\NJLearner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB406B5-C578-4317-9869-66C72D19CBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41ACAB2-1D72-47D4-8602-4FFB6F8216B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3030" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$A$1:$C$52</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="181">
   <si>
     <t>die Katze</t>
   </si>
@@ -212,9 +215,6 @@
     <t>arbeiten</t>
   </si>
   <si>
-    <t>dělat</t>
-  </si>
-  <si>
     <t>wandern</t>
   </si>
   <si>
@@ -323,9 +323,6 @@
     <t>nehmen</t>
   </si>
   <si>
-    <t>ambieten</t>
-  </si>
-  <si>
     <t>nabídnout</t>
   </si>
   <si>
@@ -347,9 +344,6 @@
     <t>bringen</t>
   </si>
   <si>
-    <t>ochutnávat</t>
-  </si>
-  <si>
     <t>schmecken</t>
   </si>
   <si>
@@ -390,6 +384,249 @@
   </si>
   <si>
     <t>verbs</t>
+  </si>
+  <si>
+    <t>ziehen</t>
+  </si>
+  <si>
+    <t>dostat</t>
+  </si>
+  <si>
+    <t>bekommen</t>
+  </si>
+  <si>
+    <t>pracovat</t>
+  </si>
+  <si>
+    <t>anbieten</t>
+  </si>
+  <si>
+    <t>ochutnat</t>
+  </si>
+  <si>
+    <t>ukázat</t>
+  </si>
+  <si>
+    <t>začínat</t>
+  </si>
+  <si>
+    <t>končit</t>
+  </si>
+  <si>
+    <t>dávat pozor</t>
+  </si>
+  <si>
+    <t>měl by</t>
+  </si>
+  <si>
+    <t>zopakovat</t>
+  </si>
+  <si>
+    <t>hledat</t>
+  </si>
+  <si>
+    <t>zapomenout</t>
+  </si>
+  <si>
+    <t>připravovat</t>
+  </si>
+  <si>
+    <t>opravovat</t>
+  </si>
+  <si>
+    <t>číst</t>
+  </si>
+  <si>
+    <t>rozumět/chápat</t>
+  </si>
+  <si>
+    <t>myslet</t>
+  </si>
+  <si>
+    <t>zotročit</t>
+  </si>
+  <si>
+    <t>psát</t>
+  </si>
+  <si>
+    <t>odpovídat</t>
+  </si>
+  <si>
+    <t>řešit</t>
+  </si>
+  <si>
+    <t>zpívat</t>
+  </si>
+  <si>
+    <t>chtít</t>
+  </si>
+  <si>
+    <t>doporučit</t>
+  </si>
+  <si>
+    <t>vybrat</t>
+  </si>
+  <si>
+    <t>pít</t>
+  </si>
+  <si>
+    <t>objednat</t>
+  </si>
+  <si>
+    <t>slavit</t>
+  </si>
+  <si>
+    <t>pobývat</t>
+  </si>
+  <si>
+    <t>doplnit/přidat</t>
+  </si>
+  <si>
+    <t>přemístit</t>
+  </si>
+  <si>
+    <t>vypadat/vyhlížet</t>
+  </si>
+  <si>
+    <t>vést</t>
+  </si>
+  <si>
+    <t>spát</t>
+  </si>
+  <si>
+    <t>stát/vydržet</t>
+  </si>
+  <si>
+    <t>odložit si/vykonat</t>
+  </si>
+  <si>
+    <t>sedět</t>
+  </si>
+  <si>
+    <t>vědět</t>
+  </si>
+  <si>
+    <t>platit</t>
+  </si>
+  <si>
+    <t>pomáhat</t>
+  </si>
+  <si>
+    <t>narodit se</t>
+  </si>
+  <si>
+    <t>beginnen</t>
+  </si>
+  <si>
+    <t>enden</t>
+  </si>
+  <si>
+    <t>aufpasen</t>
+  </si>
+  <si>
+    <t>sollen</t>
+  </si>
+  <si>
+    <t>wiederholen</t>
+  </si>
+  <si>
+    <t>suchen</t>
+  </si>
+  <si>
+    <t>vergessen</t>
+  </si>
+  <si>
+    <t>vorbereiten</t>
+  </si>
+  <si>
+    <t>korrigieren</t>
+  </si>
+  <si>
+    <t>lesen</t>
+  </si>
+  <si>
+    <t>verstehen</t>
+  </si>
+  <si>
+    <t>denken</t>
+  </si>
+  <si>
+    <t>erkläven</t>
+  </si>
+  <si>
+    <t>schreiben</t>
+  </si>
+  <si>
+    <t>antworten</t>
+  </si>
+  <si>
+    <t>sdělit</t>
+  </si>
+  <si>
+    <t>erzahlen</t>
+  </si>
+  <si>
+    <t>lösen</t>
+  </si>
+  <si>
+    <t>singen</t>
+  </si>
+  <si>
+    <t>wollen</t>
+  </si>
+  <si>
+    <t>empfehlen</t>
+  </si>
+  <si>
+    <t>wählen</t>
+  </si>
+  <si>
+    <t>trinken</t>
+  </si>
+  <si>
+    <t>bestellen</t>
+  </si>
+  <si>
+    <t>feiern</t>
+  </si>
+  <si>
+    <t>bleiben</t>
+  </si>
+  <si>
+    <t>ergänzen</t>
+  </si>
+  <si>
+    <t>umziehen</t>
+  </si>
+  <si>
+    <t>aussehen</t>
+  </si>
+  <si>
+    <t>führen</t>
+  </si>
+  <si>
+    <t>schlafen</t>
+  </si>
+  <si>
+    <t>stehen</t>
+  </si>
+  <si>
+    <t>ablegen</t>
+  </si>
+  <si>
+    <t>sitzen</t>
+  </si>
+  <si>
+    <t>wissen</t>
+  </si>
+  <si>
+    <t>bezahlen</t>
+  </si>
+  <si>
+    <t>helfen</t>
+  </si>
+  <si>
+    <t>geboren</t>
   </si>
 </sst>
 </file>
@@ -728,15 +965,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -781,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,7 +1074,7 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -848,7 +1085,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,7 +1096,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,7 +1107,7 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,7 +1118,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,7 +1129,7 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,7 +1140,7 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,7 +1151,7 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -925,7 +1162,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -936,7 +1173,7 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,7 +1184,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,340 +1195,770 @@
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
         <v>100</v>
       </c>
-      <c r="B50" t="s">
-        <v>101</v>
-      </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>152</v>
+      </c>
+      <c r="C62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>158</v>
+      </c>
+      <c r="B68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" t="s">
+        <v>161</v>
+      </c>
+      <c r="C70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" t="s">
+        <v>162</v>
+      </c>
+      <c r="C71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" t="s">
+        <v>166</v>
+      </c>
+      <c r="C75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" t="s">
+        <v>168</v>
+      </c>
+      <c r="C77" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>131</v>
+      </c>
+      <c r="B78" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>132</v>
+      </c>
+      <c r="B79" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>133</v>
+      </c>
+      <c r="B80" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" t="s">
+        <v>172</v>
+      </c>
+      <c r="C81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>135</v>
+      </c>
+      <c r="B82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>136</v>
+      </c>
+      <c r="B83" t="s">
+        <v>174</v>
+      </c>
+      <c r="C83" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" t="s">
+        <v>175</v>
+      </c>
+      <c r="C84" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>138</v>
+      </c>
+      <c r="B85" t="s">
+        <v>176</v>
+      </c>
+      <c r="C85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>142</v>
+      </c>
+      <c r="B89" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>